<commit_message>
change T9 into DSP and increase task fps by one third
</commit_message>
<xml_diff>
--- a/doc/argument.xlsx
+++ b/doc/argument.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\workspace\ai_scheduler\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workspace\ai_scheduler\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C9B8F-38DA-4FC9-9BBD-2F752658367A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E536D7-4016-4969-942F-A59CA6B3632B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Task</t>
   </si>
@@ -39,16 +28,10 @@
     <t>NPU</t>
   </si>
   <si>
-    <t>NPU BW</t>
-  </si>
-  <si>
     <t>DSP</t>
   </si>
   <si>
     <t>System</t>
-  </si>
-  <si>
-    <t>NPU Real</t>
   </si>
   <si>
     <t>75.50%</t>
@@ -59,6 +42,18 @@
   </si>
   <si>
     <t>TK Task[1:8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TK Task[1:8]+T9 on NPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPU/System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPU/DSP BW</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -469,48 +464,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1"/>
-    <col min="4" max="5" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="23.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3">
         <v>0.69799999999999995</v>
-      </c>
-      <c r="C2" s="2">
-        <v>40</v>
       </c>
       <c r="D2" s="3">
         <v>0.41299999999999998</v>
@@ -519,233 +515,246 @@
         <v>0.86499999999999999</v>
       </c>
       <c r="F2" s="3">
-        <f>B2/E2</f>
+        <f>C2/E2</f>
         <v>0.80693641618497103</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3">
         <v>0.69799999999999995</v>
-      </c>
-      <c r="C3" s="2">
-        <v>40</v>
       </c>
       <c r="D3" s="3">
         <v>0.17799999999999999</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3">
-        <f>B3/E3</f>
+        <f>C3/E3</f>
         <v>0.92450331125827812</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <f>C4/E4</f>
+        <v>0.92857142857142849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="5"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1 E3" numberStoredAsText="1"/>
+    <ignoredError sqref="C1 E3 A1 D1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
increase fps by 1/3
</commit_message>
<xml_diff>
--- a/doc/argument.xlsx
+++ b/doc/argument.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workspace\ai_scheduler\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E536D7-4016-4969-942F-A59CA6B3632B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2103B851-5AD0-4279-9CE7-11687AF4B762}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Task</t>
   </si>
@@ -54,6 +54,22 @@
   </si>
   <si>
     <t>NPU/DSP BW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>TK Task[1:8]+T9 on NPU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>全体膨胀约1/3</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -61,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +97,13 @@
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -464,13 +487,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.75" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.25" style="1" bestFit="1" customWidth="1"/>
@@ -561,13 +584,26 @@
         <v>0.92857142857142849</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="F5" s="3">
+        <f>C5/E5</f>
+        <v>0.96845425867507895</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>

</xml_diff>